<commit_message>
Updated app.py and chatbot_responses
</commit_message>
<xml_diff>
--- a/chatbot_responses.xlsx
+++ b/chatbot_responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\OneDrive\Desktop\ChatBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B0218-1B12-4EAF-A2CF-C8E6FAE9A0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76845C51-DC90-4EF7-AD65-5E79A121CFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="2340" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
-    <t>User_Input</t>
-  </si>
-  <si>
-    <t>Bot_Response</t>
-  </si>
-  <si>
     <t>hello</t>
   </si>
   <si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t>appraisal report</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Response</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,66 +404,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the responses sheet
</commit_message>
<xml_diff>
--- a/chatbot_responses.xlsx
+++ b/chatbot_responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\OneDrive\Desktop\ChatBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA8DA62-DC50-4C34-9BA6-3F654662E39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516C3E3D-2A7C-4B96-A999-B6D5AAF60AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="199">
   <si>
     <t>hello</t>
   </si>
@@ -402,53 +402,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>After log in in to Parichay from the left side menu panel select "Workflow", and then "Create/Update Workflow".  And then search by employee name or Employee ID.  Click on "Create Workflow".  Select correct Assessment period.  Select APAR/NRC as applicable. Select correct form type.  click “Action” button and then "Continue".  Here select correct reporting authority by search  option on the right side.  New window for search will open.  In the search window  “service” to be chosen as  INCOME TAX (GZTD) if your reporting officer is Group B Gazetted officer and " INCOME TAX REVENUE SERVICE (IT)" if your reporting officer is IRS officer . Give input as name or employee code and press  “search”. From the search result select your reporting officer. Choose reviewing officer in the same method.  Click “save” (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>do not press “save and next”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">) .  You will see comment </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Workflow has been created successfully"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in a new window. </t>
-    </r>
-  </si>
-  <si>
     <t>How to initiate NRC</t>
   </si>
   <si>
@@ -1108,9 +1061,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Is it compulsory to fill IPR </t>
-  </si>
-  <si>
     <t>All the officers and officials from the APAR year 2024-25 have to compulsorily fill APAR online in SPARROW portal.</t>
   </si>
   <si>
@@ -1135,25 +1085,85 @@
     <t>The IPR i.e., Immovable Property Return has to be submitted by all officers up to the cadres of Group B Non Gazetted compulsorily  before 31st January every year  with details of immovable property held as on 01st January of that year.</t>
   </si>
   <si>
+    <t>Is it compulsory to fill Immovable Property Return</t>
+  </si>
+  <si>
+    <t>sparrow</t>
+  </si>
+  <si>
+    <r>
+      <t>1. After log in in to Parichay from the left side menu panel select "Workflow" and then "Create/Update Workflow" &lt;br&gt;&lt;br&gt;2. Search by employee name or Employee ID.  Click on "Create Workflow".&lt;br&gt;&lt;br&gt;3.  Select correct Assessment period.&lt;br&gt;&lt;br&gt;3. Select APAR/NRC as applicable.&lt;br&gt;&lt;br&gt;4. Select correct form type.&lt;br&gt;&lt;br&gt;5. Click “Action” button and then "Continue".  Here select correct reporting authority by search  option on the right side.  New window for search will open. &lt;br&gt;&lt;br&gt;6. In the search window  “service” to be chosen as  INCOME TAX (GZTD) if your reporting officer is Group B Gazetted officer and " INCOME TAX REVENUE SERVICE (IT)" if your reporting officer is IRS officer . Give input as name or employee code and press  “search”. From the search result select your reporting officer. Choose reviewing officer in the same method.  Click “save” (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>do not press “save and next”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) .  You will see comment </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Workflow has been created successfully"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in a new window. </t>
+    </r>
+  </si>
+  <si>
+    <t>not able to login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is it compulsory to file IPR </t>
+  </si>
+  <si>
     <t>Yes.  The IPR has to be filed by all officers up to the cadres of Group B Non Gazetted compulsorily  before 31st January every year  with details of immovable property held as on 01st January of that year.
-Rule 18(1)(ii) of the CCS (Conduct) Rules, 1964 states as under: 
+Rule 18(1)(ii) of the CCS (Conduct) Rules, 1964 states as under:&lt;br&gt;&lt;br&gt; 
 “(ii) Every Government servant belonging to any service or holding any post included in Group ‘A’ and Group ‘B’ shall submit an annual return in such form as may be prescribed by the Government in this regard giving full particulars regarding the immovable property inherited by him or owned or acquired by him or held by him on lease or mortgage either in his own name or in the name of any member of his family or in the name of any other person.” 
 Accordingly, all Group 'A' and Group 'B' Government servants are required to file Annual Immovable Property Return (IPR) of the previous year latest by 31st January of the following year. 
-Kind attention is also invited to DoPT OM No. 104/33/2024-A VD-IA dated 09.10.2024, which states that vigilance clearance shall be denied to an officer, if he/she fails to submit his/her annual immovable property return of the previous year by 31st January of the following year in the following cases: 
-I. Empanelment 
-ii. Ex- India study leave 
-iii. Any deputation for which clearance is necessary and extension there of 
-iv. Appointment to sensitive posts. 
-v. Assignments to training programmes except mandatory training 
-vi. Confirmation in service 
-vii. Retirement on VRS 
-viii. Post-retirement commercial employment 
-ix. Pre-mature repatriation (voluntary) from any deputation 
+&lt;br&gt;&lt;br&gt;
+Kind attention is also invited to DoPT OM No. 104/33/2024-A VD-IA dated 09.10.2024, which states that vigilance clearance shall be denied to an officer, if he/she fails to submit his/her annual immovable property return of the previous year by 31st January of the following year in the following cases:&lt;br&gt;&lt;br&gt; 
+I. Empanelment&lt;br&gt;&lt;br&gt; 
+ii. Ex- India study leave&lt;br&gt;&lt;br&gt; 
+iii. Any deputation for which clearance is necessary and extension there of &lt;br&gt;&lt;br&gt; 
+iv. Appointment to sensitive posts. &lt;br&gt;&lt;br&gt; 
+v. Assignments to training programmes except mandatory training &lt;br&gt;&lt;br&gt; 
+vi. Confirmation in service &lt;br&gt;&lt;br&gt; 
+vii. Retirement on VRS &lt;br&gt;&lt;br&gt; 
+viii. Post-retirement commercial employment &lt;br&gt;&lt;br&gt; 
+ix. Pre-mature repatriation (voluntary) from any deputation &lt;br&gt;&lt;br&gt; 
 Kind attention is also drawn to, the Central Vigilance Commission's Office Order No. 17/11/2020 dated 23.11.2020, circulated vide this Office letter F.No. P 329/Personnel/IPR/2020-21/754 dated 18.12.2020, mentioning that timely filing of Property Return by the officials of Ministries/Departments/Organizations is one of the mandatory requirement under CCS (Conduct) Rules and non-filing of Property Returns constitutes good and sufficient reasons for instituting disciplinary action against the delinquent officials. 
 Therefore, filing of IPR is very important for all Group-A and Group-B Government servants</t>
   </si>
   <si>
-    <t>Is it compulsory to fill Immovable Property Return</t>
+    <t xml:space="preserve">IPR is to be filed in SPARROW portal.&lt;br&gt;&lt;br&gt;1.Log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt;  with sparrow id, password and OTP. The SPARROW/Parichay opens.&lt;br&gt;&lt;br&gt; 2.Again log in in this page with same SPARROW User ID and Password and newly generated OTP.&lt;br&gt;&lt;br&gt;3. When the new page is opened select and click on Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable.  &lt;br&gt;&lt;br&gt;4. On the left bottom of the panel IPR appear.  File the IPR either filling on line or uploading presigned PDF of the IPR return. </t>
   </si>
 </sst>
 </file>
@@ -1578,10 +1588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R158"/>
+  <dimension ref="A1:R160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1658,7 +1668,7 @@
     </row>
     <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>74</v>
@@ -1674,10 +1684,10 @@
     </row>
     <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1685,7 +1695,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -1722,7 +1732,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>71</v>
@@ -1738,7 +1748,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>62</v>
@@ -1746,15 +1756,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>63</v>
@@ -1762,15 +1772,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>64</v>
@@ -1778,71 +1788,71 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>65</v>
@@ -1850,31 +1860,31 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>67</v>
@@ -1882,167 +1892,167 @@
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>179</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="B41" s="1" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="B45" s="1" t="s">
-        <v>182</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="237" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>183</v>
+        <v>49</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="237" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="237" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>69</v>
+      <c r="B56" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>69</v>
@@ -2050,715 +2060,723 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>80</v>
+      <c r="B62" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>186</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>187</v>
+        <v>91</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>93</v>
+        <v>185</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>95</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>188</v>
+        <v>97</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>99</v>
+        <v>186</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>189</v>
+        <v>100</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
-        <v>190</v>
+        <v>101</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B106" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="7" t="s">
+      <c r="B108" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B128" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="6" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="6" t="s">
-        <v>159</v>
-      </c>
       <c r="B129" s="6" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B136" s="8" t="s">
-        <v>194</v>
+        <v>163</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B138" s="6" t="s">
-        <v>167</v>
+        <v>196</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B143" s="8" t="s">
-        <v>194</v>
+        <v>171</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A145" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B146" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B144" s="6" t="s">
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="6"/>
-      <c r="B146" s="6"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="6"/>
-      <c r="B147" s="6"/>
+      <c r="B147" s="6" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="6"/>
@@ -2803,6 +2821,14 @@
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified the responses sheet form adjusted
</commit_message>
<xml_diff>
--- a/chatbot_responses.xlsx
+++ b/chatbot_responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\OneDrive\Desktop\ChatBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516C3E3D-2A7C-4B96-A999-B6D5AAF60AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DD49C4-A9EB-4174-9830-21C3F370DA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,9 +222,6 @@
     <t>No Report Certificate</t>
   </si>
   <si>
-    <t xml:space="preserve">Form is selected while initiating APAR work flow basing on the duties assigned i.e., Faceless or .  </t>
-  </si>
-  <si>
     <t xml:space="preserve">A Basic Information form is to be filled by ORU manually with self signature and to be attested by DDO and to be handed over to concerned PAR Manager for filling the details in Basic Information page of APAR.  PAR Manager fills the Basic Information and e-signs in sparrow portal.  Then the APAR is automatically shifted to ORU console for Self Appraisal. </t>
   </si>
   <si>
@@ -1164,6 +1161,9 @@
   </si>
   <si>
     <t xml:space="preserve">IPR is to be filed in SPARROW portal.&lt;br&gt;&lt;br&gt;1.Log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt;  with sparrow id, password and OTP. The SPARROW/Parichay opens.&lt;br&gt;&lt;br&gt; 2.Again log in in this page with same SPARROW User ID and Password and newly generated OTP.&lt;br&gt;&lt;br&gt;3. When the new page is opened select and click on Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable.  &lt;br&gt;&lt;br&gt;4. On the left bottom of the panel IPR appear.  File the IPR either filling on line or uploading presigned PDF of the IPR return. </t>
+  </si>
+  <si>
+    <t>Form is selected while initiating APAR work flow basing on the duties assigned i.e., Faceless or Jurisdictional or Central or International Taxation or Other than assessment duties.</t>
   </si>
 </sst>
 </file>
@@ -1590,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1645,7 +1645,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -1653,7 +1653,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -1663,15 +1663,15 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -1679,15 +1679,15 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1695,31 +1695,31 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1727,15 +1727,15 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1743,12 +1743,12 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>62</v>
@@ -1796,10 +1796,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1807,7 +1807,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1815,7 +1815,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1823,7 +1823,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1831,7 +1831,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1839,7 +1839,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1847,7 +1847,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1855,7 +1855,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1863,7 +1863,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>65</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1871,7 +1871,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1879,7 +1879,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1887,7 +1887,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1895,7 +1895,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1903,7 +1903,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1911,7 +1911,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1919,15 +1919,15 @@
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1935,7 +1935,7 @@
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1943,7 +1943,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1951,7 +1951,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1959,7 +1959,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1967,15 +1967,15 @@
         <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1983,7 +1983,7 @@
         <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1991,7 +1991,7 @@
         <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1999,7 +1999,7 @@
         <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2007,7 +2007,7 @@
         <v>46</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2015,7 +2015,7 @@
         <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -2023,7 +2023,7 @@
         <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -2031,7 +2031,7 @@
         <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="237" x14ac:dyDescent="0.3">
@@ -2039,7 +2039,7 @@
         <v>50</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="237" x14ac:dyDescent="0.3">
@@ -2047,7 +2047,7 @@
         <v>51</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -2055,7 +2055,7 @@
         <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -2063,7 +2063,7 @@
         <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -2071,7 +2071,7 @@
         <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -2079,7 +2079,7 @@
         <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -2087,7 +2087,7 @@
         <v>56</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
@@ -2095,7 +2095,7 @@
         <v>57</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -2103,7 +2103,7 @@
         <v>58</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -2111,7 +2111,7 @@
         <v>59</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -2119,7 +2119,7 @@
         <v>60</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -2135,647 +2135,647 @@
         <v>61</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B92" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B114" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B117" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B121" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="B121" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B122" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B125" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B128" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B138" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B139" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="B139" s="6" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B141" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="B141" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B146" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="B146" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated the data dictionary
</commit_message>
<xml_diff>
--- a/chatbot_responses.xlsx
+++ b/chatbot_responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\OneDrive\Desktop\ChatBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DD49C4-A9EB-4174-9830-21C3F370DA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A6D9E4-76F1-4DD4-A056-5431022633DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="314">
   <si>
     <t>hello</t>
   </si>
@@ -214,12 +214,6 @@
   </si>
   <si>
     <t>Smart Performance Appraisal Report Recording Online Window</t>
-  </si>
-  <si>
-    <t>Annual Performance Appraisal Report</t>
-  </si>
-  <si>
-    <t>No Report Certificate</t>
   </si>
   <si>
     <t xml:space="preserve">A Basic Information form is to be filled by ORU manually with self signature and to be attested by DDO and to be handed over to concerned PAR Manager for filling the details in Basic Information page of APAR.  PAR Manager fills the Basic Information and e-signs in sparrow portal.  Then the APAR is automatically shifted to ORU console for Self Appraisal. </t>
@@ -642,9 +636,6 @@
     <t>is it necessary to upload document</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes.  The supporting document for NRC request has to be uploaded compulsorily.  Upload the document in “Reference Upload” (only PDF files with 3 mb maximum size).  The documents are  Reporting officer’s CTC/ Self CTC/ Self Transfer order/ Promotion order/ approved leave application of more than 15 days/ joining time entry in Service register so on … which ever is applicable. </t>
-  </si>
-  <si>
     <t>Upload document</t>
   </si>
   <si>
@@ -949,9 +940,6 @@
   </si>
   <si>
     <t>Do I need to submit IPR copy</t>
-  </si>
-  <si>
-    <t>No.  You need not submit copy of the Immovable Property Return anywhere once submitted in SPARROW portal.</t>
   </si>
   <si>
     <t>Where to submit copy of IPR</t>
@@ -1141,7 +1129,16 @@
     <t xml:space="preserve">Is it compulsory to file IPR </t>
   </si>
   <si>
-    <t>Yes.  The IPR has to be filed by all officers up to the cadres of Group B Non Gazetted compulsorily  before 31st January every year  with details of immovable property held as on 01st January of that year.
+    <t xml:space="preserve">IPR is to be filed in SPARROW portal.&lt;br&gt;&lt;br&gt;1.Log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt;  with sparrow id, password and OTP. The SPARROW/Parichay opens.&lt;br&gt;&lt;br&gt; 2.Again log in in this page with same SPARROW User ID and Password and newly generated OTP.&lt;br&gt;&lt;br&gt;3. When the new page is opened select and click on Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable.  &lt;br&gt;&lt;br&gt;4. On the left bottom of the panel IPR appear.  File the IPR either filling on line or uploading presigned PDF of the IPR return. </t>
+  </si>
+  <si>
+    <t>Form is selected while initiating APAR work flow basing on the duties assigned i.e., Faceless or Jurisdictional or Central or International Taxation or Other than assessment duties.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  The supporting document for NRC request has to be uploaded compulsorily.  Upload the document in “Reference Upload” (only PDF files with 3 mb maximum size).  The documents are  Reporting officer’s CTC/ Self CTC/ Self Transfer order/ Promotion order/ approved leave application of more than 15 days/ joining time entry in Service register so on … which ever is applicable. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  The IPR has to be filed by all officers up to the cadres of Group B Non Gazetted compulsorily  before 31st January every year  with details of immovable property held as on 01st January of that year.
 Rule 18(1)(ii) of the CCS (Conduct) Rules, 1964 states as under:&lt;br&gt;&lt;br&gt; 
 “(ii) Every Government servant belonging to any service or holding any post included in Group ‘A’ and Group ‘B’ shall submit an annual return in such form as may be prescribed by the Government in this regard giving full particulars regarding the immovable property inherited by him or owned or acquired by him or held by him on lease or mortgage either in his own name or in the name of any member of his family or in the name of any other person.” 
 Accordingly, all Group 'A' and Group 'B' Government servants are required to file Annual Immovable Property Return (IPR) of the previous year latest by 31st January of the following year. 
@@ -1160,17 +1157,488 @@
 Therefore, filing of IPR is very important for all Group-A and Group-B Government servants</t>
   </si>
   <si>
-    <t xml:space="preserve">IPR is to be filed in SPARROW portal.&lt;br&gt;&lt;br&gt;1.Log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt;  with sparrow id, password and OTP. The SPARROW/Parichay opens.&lt;br&gt;&lt;br&gt; 2.Again log in in this page with same SPARROW User ID and Password and newly generated OTP.&lt;br&gt;&lt;br&gt;3. When the new page is opened select and click on Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable.  &lt;br&gt;&lt;br&gt;4. On the left bottom of the panel IPR appear.  File the IPR either filling on line or uploading presigned PDF of the IPR return. </t>
-  </si>
-  <si>
-    <t>Form is selected while initiating APAR work flow basing on the duties assigned i.e., Faceless or Jurisdictional or Central or International Taxation or Other than assessment duties.</t>
+    <t>You need not submit copy of the Immovable Property Return anywhere once submitted in SPARROW portal.</t>
+  </si>
+  <si>
+    <t>Annual Performance Appraisal Report.  The self appraisal is to be submitted before 30th Apr.</t>
+  </si>
+  <si>
+    <t>No Report Certificate.  When the ORU works under his supervisory officer for less than 90 days, NRC is to be initiated in SPARROW.</t>
+  </si>
+  <si>
+    <t>Whom should I contact</t>
+  </si>
+  <si>
+    <t>Please send your queries by mentioning your Name, Emp ID, Cadre, Present office of Posting, Mobile Number to &lt;b&gt;hyderabad.dcit.hq.vig@incometax.gov.in&lt;b&gt; (For Hyderabad region only)</t>
+  </si>
+  <si>
+    <t>Can I use my income tax mail id for sparrow</t>
+  </si>
+  <si>
+    <t>The log in id for SPARROW is separetly created and was communicated to your registered mobile number. For any queries contact  &lt;b&gt;hyderabad.dcit.hq.vig@incometax.gov.in&lt;b&gt; (For Hyderabad region only) by mentioning your Name, Emp ID, Cadre, Present office of Posting, Mobile Number.</t>
+  </si>
+  <si>
+    <t>How to delete wrongly created APAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The wrongly created APAR can be deleted by the PAR Manager upto the stage before e sign.  Once the PAR Manager esigns, it has to be deleted by Primary Custodian only.  Please send the details of PAR period to &lt;b&gt;&lt;b&gt;hyderabad.dcit.hq.vig@incometax.gov.in&lt;b&gt; (For Hyderabad region only)&lt;b&gt; with details of ORU such as Name, Emp ID, Cadre, Present office of Posting, Mobile Number to </t>
+  </si>
+  <si>
+    <t>Delete workflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The wrongly created APAR can be deleted by the PAR Manager upto the stage before e sign.  Once the PAR Manager esigns, it has to be deleted by Primary Custodian only.  Please send the details of PAR period to &lt;b&gt;hyderabad.dcit.hq.vig@incometax.gov.in&lt;b&gt; (For Hyderabad region only) with details of ORU such as Name, Emp ID, Cadre, Present office of Posting, Mobile Number to </t>
+  </si>
+  <si>
+    <t>wrong apar</t>
+  </si>
+  <si>
+    <t>How to submit apar</t>
+  </si>
+  <si>
+    <t>Stage 1 :  Log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt; with SPARROW id, password and OTP → log in to SPARROW/parichay with SPARROW id, password and OTP → select Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable → select “User Assistance” → select “Create Self Workflow” → create workflow → chose Organisation Posted as CBDT IT AP&amp; Telangana → select period → select APAR/NRC as applicable → select “form type” → select “Action” → select “continue” → select correct reporting authority by search   option → In “service” column choose INCOME TAX (GZTD) or INCOME TAX REVENUE SERVICE (IT) as applicable → give input as name or employee code and click on “search” → select your reporting officer → choose reviewing officer in the same method → click “save” (do not press “save and next”) → you will see comment  Workflow has been created successfully  in a new window → fill manual basic information form, put your signature → get your DDO signature → hand over to your PAR Manager.&lt;br&gt;&lt;br&gt;  
+ Stage 2 : When your par manager e-signs your par, log in to SPARROW as above → go to inbox → click on My PAR → you will be directed to self appraisal page → write your ‘self appraisal’ → click on Send to Reporting Officer&lt;br&gt;&lt;br&gt; 
+Stage 3: After completion of Reporting Officer and Reviewing officer comments the CR Section will send your APAR back to you for acceptance → Log in to https://saccess.nic with SPARROW id, password and OTP → log in to SPARROW/parichay with SPARROW id, password and OTP → select Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable → click on “My PAR” → click the pending APAR → click on Officer Discloser → click on Accept if satisfied or file your representation if not satisfied → sign digitally by DSC or e-Hastakshar.</t>
+  </si>
+  <si>
+    <t>What are the necessary documents to be uploaded for NRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The supporting document for NRC request has to be uploaded compulsorily.  Upload the document in “Reference Upload” (only PDF files with 3 MB maximum size).  The documents are  Reporting officer’s CTC/ Self CTC/ Self Transfer order/ Promotion order/ approved leave application of more than 15 days/ joining time entry in Service register so on … which ever is applicable. </t>
+  </si>
+  <si>
+    <t>Necessary documents for NRC</t>
+  </si>
+  <si>
+    <t>Can reviewing officer report the apar</t>
+  </si>
+  <si>
+    <t>The ORU has to submit the APAR with in stipulated time i.e., 30 Apr for APAR and with in 15 days of change of reporting officer.  Failure in not creating self work flow/submitting self appraisal within the time lines, an explanation for not having performed the public duty of writing the APAR within the due date shall be called for and a written warning shall be issued to the officer by competent authority and same will be placed in APAR dossier.  In the case where Reporting Officer has not reported with in the stipulated time the APAR will be been force forwarded to Reviewing officer by the competent authrity and APAR is reviewed by Reviewing Officer and  an explanation for not having performed the public duty of reporting the APAR within the due date shall be called for from the Reporting Officer by competent authority and same will be placed in APAR dossier.</t>
+  </si>
+  <si>
+    <t>What is SPARROW id</t>
+  </si>
+  <si>
+    <t>The SPARROW ID is allocated by HRD, CBDT consisting of your part name and employee number and is linked with registred mobile number.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPARROW email </t>
+  </si>
+  <si>
+    <t>How to get SPARROW id</t>
+  </si>
+  <si>
+    <t>By default all the officers/officials are allocated with sparrow id. The newly joined officials have to send their details  by mentioning their Name, Emp ID, Cadre, Present office of Posting, Mobile Number to &lt;b&gt;hyderabad.dcit.hq.vig@incometax.gov.in&lt;b&gt; (For Hyderabad region only).</t>
+  </si>
+  <si>
+    <t>How to generate SPARROW id</t>
+  </si>
+  <si>
+    <t>By default all the officers/officials are allocated with sparrow id. The newly joined officials have to send their details  by mentioning their Name, Emp ID, Cadre, Present office of Posting, Mobile Number to &lt;b&gt;hyderabad.dcit.hq.vig@incometax.gov.in&lt;b&gt; (For Hyderabad region only) .</t>
+  </si>
+  <si>
+    <t>Where do I find my SPARROW credentials</t>
+  </si>
+  <si>
+    <t>Sparrow credentials are shared by HRD, CBDT to your registered mobile number.  In case forgotten please send your queries by mentioning your Name, Emp ID, Cadre, Present office of Posting, Mobile Number to &lt;b&gt;hyderabad.dcit.hq.vig@incometax.gov.in&lt;b&gt; (For Hyderabad region only)</t>
+  </si>
+  <si>
+    <t>Who neeeds a SPARROW id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All the officers for filing APAR, NRC and IPR online are required with Sparrow credentials. </t>
+  </si>
+  <si>
+    <t>Why do we need a SPPROW id</t>
+  </si>
+  <si>
+    <t>Whom to contact if there is no SPARROW id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default all the officers/officials are allocated with sparrow id. The newly joined officials have to send their details  by mentioning their Name, Emp ID, Cadre, Present office of Posting, Mobile Number to &lt;b&gt;hyderabad.dcit.hq.vig@incometax.gov.in&lt;b&gt; (For Hyderabad region only) </t>
+  </si>
+  <si>
+    <t>Who is custodian of APAR</t>
+  </si>
+  <si>
+    <t>Dy Commissioner of Income Tax (HQrs) (Vigelance), Hyderabad is the Primary Custodian of APAR</t>
+  </si>
+  <si>
+    <t>Alternate custodian</t>
+  </si>
+  <si>
+    <t>How to check the status of APAR</t>
+  </si>
+  <si>
+    <t>Log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt; with SPARROW id, password and OTP → log in to SPARROW/parichay with SPARROW id, password and OTP → select Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable → click on “My PAR”</t>
+  </si>
+  <si>
+    <t>status of APAR</t>
+  </si>
+  <si>
+    <t>Where is my APAR</t>
+  </si>
+  <si>
+    <t>Creation of self workflow</t>
+  </si>
+  <si>
+    <t>How to create workflow</t>
+  </si>
+  <si>
+    <t>Who should create workflow</t>
+  </si>
+  <si>
+    <t>Workflow has to be created by ORU him/herself by login to SPARROW portal.</t>
+  </si>
+  <si>
+    <t>What is to be choosen in Organisation posted while creating workflow</t>
+  </si>
+  <si>
+    <t>For AP&amp; Telangana charge CBDT IT AP&amp; Telangana is to be choosen as organisation</t>
+  </si>
+  <si>
+    <t>what is Organisation posted</t>
+  </si>
+  <si>
+    <t>Which one to select for Organisation posted</t>
+  </si>
+  <si>
+    <t>Who can delete the workflow already created</t>
+  </si>
+  <si>
+    <t>Can I delete Workflow already created</t>
+  </si>
+  <si>
+    <t>Can I make changes in Workflow</t>
+  </si>
+  <si>
+    <t>How to update workflow</t>
+  </si>
+  <si>
+    <t>How to make changes in Workflow</t>
+  </si>
+  <si>
+    <t>How to delete created workflow</t>
+  </si>
+  <si>
+    <t>Wat is APAR Formtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For writing APAR different forms have been prescribed for different duties assigned.  Such as Faceless, Jurisdictional, International Taxation, Audit, otherthan assessment duties, Administrative Officer/Office Superintendent, Private Secretary/Stenographer so on.  While initiating workflow, correct form is to be choosen. </t>
+  </si>
+  <si>
+    <t>Form Type APAR</t>
+  </si>
+  <si>
+    <t>How to select Form type</t>
+  </si>
+  <si>
+    <t>How to select reporting authority</t>
+  </si>
+  <si>
+    <t>Reporting authority search</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select correct reporting authority by search  option </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> In “service” column choose INCOME TAX (GZTD) or INCOME TAX REVENUE SERVICE (IT) as applicable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">→ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">give input as name or employee code and click on “search” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> select your reporting officer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>→</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> choose reviewing officer in the same method </t>
+    </r>
+  </si>
+  <si>
+    <t>How to select reviewing authority</t>
+  </si>
+  <si>
+    <t>Reviewing authority search</t>
+  </si>
+  <si>
+    <t>Basic Information in APAR</t>
+  </si>
+  <si>
+    <t>How to edit basic information</t>
+  </si>
+  <si>
+    <t>Correction of basic information can be done by Primary Custodian. While initiating APAR completeness and accuracy is necessary</t>
+  </si>
+  <si>
+    <t>Can I update basic information</t>
+  </si>
+  <si>
+    <t>Can I make changes in basic information after submission</t>
+  </si>
+  <si>
+    <t>How do I correct the errors in basic information after filling</t>
+  </si>
+  <si>
+    <t>Present Grade and date of continuous appointment to it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present Grade means the present cadre and the date of promotion to the present cadre. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What should I fill for Grade </t>
+  </si>
+  <si>
+    <t>What to write in Present Grade</t>
+  </si>
+  <si>
+    <t>how to file representation for filed APAR</t>
+  </si>
+  <si>
+    <t>When the APAR is disclosed to ORU after reviewing officer comments by Primary Custodian, it the ORU is not satisfied with the grading given by reporting authority, he/she can file representation in the SPARROW portal with in 15 days for disclosure of APAR to the ORU.</t>
+  </si>
+  <si>
+    <t>When to file representation</t>
+  </si>
+  <si>
+    <t>Who should I file the APAR when there are Multiple reporting and multiple reviewing officers</t>
+  </si>
+  <si>
+    <t>ORU has to initate APAR workflow if he has worked under a reporting officer more than 90 days and on every change of reporting officer.  For multiple Reveiwing officers the ORU has to : 1. If there are multiple reviewing officers available for the period of APAR, the reviewing officer who held the office for more than 90 days has to be selected.  2. If there are multiple reviewing officers available for the period of APAR, and each reviewing officer held the office for more than 90 days, then the recent reviewing officer has to be selected for reviewing the APAR for that period. 3. If there are multiple reviewing officers, and no reviewing officer held the office for more than 90 days, then the APAR need not be reviewed and  while searching the reviewing officer in the service column “No Service” and in Code  “12345TEMP “  has to be selected</t>
+  </si>
+  <si>
+    <t>Whom should I file the APAR if there are Multiple reporting officers greater than 90 days</t>
+  </si>
+  <si>
+    <t>Whom should I file the APAR if there are Multiple reporting officers less than 90 days</t>
+  </si>
+  <si>
+    <t>For the period less than 90 days worked under reporting officer, the ORU has to get NRC initiated by his PAR Manager.</t>
+  </si>
+  <si>
+    <t>Multiple reporting and one reviewing officer</t>
+  </si>
+  <si>
+    <t>ORU has to initate APAR workflow if he has worked under a reporting officer more than 90 days and on every change of reporting officer</t>
+  </si>
+  <si>
+    <t>One reporting officer and mulitple reviewing officers</t>
+  </si>
+  <si>
+    <t>How to apply for NRC</t>
+  </si>
+  <si>
+    <t>When to apply for NRC</t>
+  </si>
+  <si>
+    <r>
+      <t>Where the ORU worked under reporting officer for less than 90 days.&lt;br&gt;&lt;br&gt; 
+•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transfer of Officer Reported Upon (ORU) &lt;br&gt;&lt;br&gt; 
+•Transfer of Reporting Officer &lt;br&gt;&lt;br&gt; 
+•Retirement of Reporting Officer/ORU &lt;br&gt;&lt;br&gt; 
+•Period of leave/training for more than 15 days and when such leave/training period is deducted from the period worked under Reporting Officer becomes less than 90 days. &lt;br&gt;&lt;br&gt; 
+•Period of leave availed by Reporting Officer more than 15 days and such leave period is deducted from the entire period worked under reporting officer becomes less than 90 days.</t>
+    </r>
+  </si>
+  <si>
+    <t>What documents are to be enclosed while filing NRC</t>
+  </si>
+  <si>
+    <t>What if APAR is not filed on time</t>
+  </si>
+  <si>
+    <t>What is the process to file APAR</t>
+  </si>
+  <si>
+    <t>Stage 1 :  Log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt; with SPARROW id, password and OTP → log in to SPARROW/parichay with SPARROW id, password and OTP → select Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable → select “User Assistance” → select “Create Self Workflow” → create workflow → chose Organisation Posted as CBDT IT AP&amp; Telangana → select period → select APAR/NRC as applicable → select “form type” → select “Action” → select “continue” → select correct reporting authority by search   option → In “service” column choose INCOME TAX (GZTD) or INCOME TAX REVENUE SERVICE (IT) as applicable → give input as name or employee code and click on “search” → select your reporting officer → choose reviewing officer in the same method → click “save” (do not press “save and next”) → you will see comment  Workflow has been created successfully  in a new window → fill manual basic information form, put your signature → get your DDO signature → hand over to your PAR Manager. &lt;br&gt;&lt;br&gt; 
+ Stage 2 : When your par manager e-signs your par, log in to SPARROW as above → go to inbox → click on My PAR → you will be directed to self appraisal page → write your ‘self appraisal’ → click on Send to Reporting Officer&lt;br&gt;&lt;br&gt; 
+Stage 3: After completion of Reporting Officer and Reviewing officer comments the CR Section will send your APAR back to you for acceptance → Log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt; with SPARROW id, password and OTP → log in to SPARROW/parichay with SPARROW id, password and OTP → select Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable → click on “My PAR” → click the pending APAR → click on Officer Discloser → click on Accept if satisfied or file your representation if not satisfied → sign digitally by DSC or e-Hastakshar.</t>
+  </si>
+  <si>
+    <t>How to file the APAR</t>
+  </si>
+  <si>
+    <t>How to download APAR</t>
+  </si>
+  <si>
+    <t>When the APAR is disclosed to ORU after reviewing officer comments by Primary Custodian, the ORU can download the APAR from My PAR option.</t>
+  </si>
+  <si>
+    <t>How to e-sign or e-hastakshar or digital sign APAR</t>
+  </si>
+  <si>
+    <t>In SPARROW the digital signature can be done by using DSC (Digital Signature Certificate) or Aadhar based e-hastakshar.</t>
+  </si>
+  <si>
+    <t>How to e-sign APAR using DSC</t>
+  </si>
+  <si>
+    <t>What is IPR</t>
+  </si>
+  <si>
+    <t>Who should file IPR online</t>
+  </si>
+  <si>
+    <t>The IPR has to be filed by all officers up to the cadres of Group B Non Gazetted compulsorily  before 31st January every year  with details of immovable property held as on 01st January of that year.
+Rule 18(1)(ii) of the CCS (Conduct) Rules, 1964 states as under:&lt;br&gt;&lt;br&gt; 
+“(ii) Every Government servant belonging to any service or holding any post included in Group ‘A’ and Group ‘B’ shall submit an annual return in such form as may be prescribed by the Government in this regard giving full particulars regarding the immovable property inherited by him or owned or acquired by him or held by him on lease or mortgage either in his own name or in the name of any member of his family or in the name of any other person.” 
+Accordingly, all Group 'A' and Group 'B' Government servants are required to file Annual Immovable Property Return (IPR) of the previous year latest by 31st January of the following year. 
+&lt;br&gt;&lt;br&gt;
+Kind attention is also invited to DoPT OM No. 104/33/2024-A VD-IA dated 09.10.2024, which states that vigilance clearance shall be denied to an officer, if he/she fails to submit his/her annual immovable property return of the previous year by 31st January of the following year in the following cases:&lt;br&gt;&lt;br&gt; 
+I. Empanelment&lt;br&gt;&lt;br&gt; 
+ii. Ex- India study leave&lt;br&gt;&lt;br&gt; 
+iii. Any deputation for which clearance is necessary and extension there of &lt;br&gt;&lt;br&gt; 
+iv. Appointment to sensitive posts. &lt;br&gt;&lt;br&gt; 
+v. Assignments to training programmes except mandatory training &lt;br&gt;&lt;br&gt; 
+vi. Confirmation in service &lt;br&gt;&lt;br&gt; 
+vii. Retirement on VRS &lt;br&gt;&lt;br&gt; 
+viii. Post-retirement commercial employment &lt;br&gt;&lt;br&gt; 
+ix. Pre-mature repatriation (voluntary) from any deputation &lt;br&gt;&lt;br&gt; 
+Kind attention is also drawn to, the Central Vigilance Commission's Office Order No. 17/11/2020 dated 23.11.2020, circulated vide this Office letter F.No. P 329/Personnel/IPR/2020-21/754 dated 18.12.2020, mentioning that timely filing of Property Return by the officials of Ministries/Departments/Organizations is one of the mandatory requirement under CCS (Conduct) Rules and non-filing of Property Returns constitutes good and sufficient reasons for instituting disciplinary action against the delinquent officials. 
+Therefore, filing of IPR is very important for all Group-A and Group-B Government servants</t>
+  </si>
+  <si>
+    <t>How to file IPR on SPARROW portal</t>
+  </si>
+  <si>
+    <t>IPR online</t>
+  </si>
+  <si>
+    <t>How to check Status of IPR filed online</t>
+  </si>
+  <si>
+    <t>Go to SPARROW portal by log in to &lt;a href="https://saccess.nic.in"&gt;https://saccess.nic.in&lt;/a&gt;  with sparrow id, password and OTP.  Then the page of SPARROW/Parichay opens.  Again log in in this page with same SPARROW User ID and Password and newly generated OTP. When the new page is opened select and click on Income Tax (Gztd), Income Tax (Non-Gztd) or IRS (IT) as applicable.   On the left bottom of the panel IPR appear.  Click on IPR and you can view the status of submission and IPR can be downloaded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If IPR is filed online, do I have to submit manual IPR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">manual IPR </t>
+  </si>
+  <si>
+    <t>IPR on SPARROW</t>
+  </si>
+  <si>
+    <t>How to e-sign or e-hastakshar IPR</t>
+  </si>
+  <si>
+    <t>How to make changes in IPR after filing</t>
+  </si>
+  <si>
+    <t>After filing IPR online in sparrow portal, changes can be done before last date for filing of IPR i.e., 31 January.  After the last date no changes can be done.</t>
+  </si>
+  <si>
+    <t>Modes of signing the APAR</t>
+  </si>
+  <si>
+    <t>Is signing necessary for submission of APAR</t>
+  </si>
+  <si>
+    <t>Time limit for IPR filing</t>
+  </si>
+  <si>
+    <t>How to download filed IPR</t>
+  </si>
+  <si>
+    <t>Who is APAR manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APAR Managers (Alternate custodians) are the Officers posted in HQrs of  CCIT/ PCIT/ CIT/ DGIT/ PDIT/ DIT offices. Competent Authority has passed an order time to time assigning the duties of PAR Managers and is circulated in website incometaxhyderabad.gov.in </t>
+  </si>
+  <si>
+    <t>Correction / deletion  of APAR can be done by Primary Custodian. But correction/deletion of NRC is to be done at HRD, CBDT New Delhi level only.  Hence, while creating NRC completeness and accuracy is necessary</t>
+  </si>
+  <si>
+    <t>How to generate APAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1259,6 +1727,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1281,7 +1762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1307,6 +1788,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1588,10 +2077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R160"/>
+  <dimension ref="A1:R229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="M210" sqref="M210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1645,7 +2134,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -1653,7 +2142,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -1663,15 +2152,15 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -1679,15 +2168,15 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1695,31 +2184,31 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1727,15 +2216,15 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1743,12 +2232,12 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>62</v>
@@ -1767,7 +2256,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1775,7 +2264,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1783,7 +2272,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1791,15 +2280,15 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1807,7 +2296,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1815,7 +2304,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1823,7 +2312,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1831,7 +2320,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1839,7 +2328,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1847,7 +2336,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1855,7 +2344,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1863,7 +2352,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1871,7 +2360,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1879,7 +2368,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1887,7 +2376,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1895,7 +2384,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1903,7 +2392,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1911,7 +2400,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1919,15 +2408,15 @@
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1935,7 +2424,7 @@
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1943,7 +2432,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1951,7 +2440,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.3">
@@ -1959,7 +2448,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1967,15 +2456,15 @@
         <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1983,7 +2472,7 @@
         <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1991,7 +2480,7 @@
         <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1999,7 +2488,7 @@
         <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2007,7 +2496,7 @@
         <v>46</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2015,7 +2504,7 @@
         <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -2023,7 +2512,7 @@
         <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -2031,7 +2520,7 @@
         <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="237" x14ac:dyDescent="0.3">
@@ -2039,7 +2528,7 @@
         <v>50</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="237" x14ac:dyDescent="0.3">
@@ -2047,7 +2536,7 @@
         <v>51</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -2055,7 +2544,7 @@
         <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -2063,7 +2552,7 @@
         <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -2071,7 +2560,7 @@
         <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -2079,7 +2568,7 @@
         <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -2087,7 +2576,7 @@
         <v>56</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
@@ -2095,7 +2584,7 @@
         <v>57</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -2103,7 +2592,7 @@
         <v>58</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -2111,7 +2600,7 @@
         <v>59</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -2119,7 +2608,7 @@
         <v>60</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -2135,703 +2624,1316 @@
         <v>61</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B138" s="8" t="s">
         <v>195</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="6"/>
-      <c r="B148" s="6"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="6"/>
-      <c r="B149" s="6"/>
+      <c r="A148" t="s">
+        <v>199</v>
+      </c>
+      <c r="B148" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A149" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="6"/>
-      <c r="B150" s="6"/>
+      <c r="A150" t="s">
+        <v>203</v>
+      </c>
+      <c r="B150" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="6"/>
-      <c r="B151" s="6"/>
+      <c r="A151" t="s">
+        <v>205</v>
+      </c>
+      <c r="B151" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="6"/>
-      <c r="B152" s="6"/>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="6"/>
-      <c r="B153" s="6"/>
+      <c r="A152" t="s">
+        <v>207</v>
+      </c>
+      <c r="B152" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>208</v>
+      </c>
+      <c r="B153" s="10" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="6"/>
-      <c r="B154" s="6"/>
+      <c r="A154" t="s">
+        <v>210</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="6"/>
-      <c r="B155" s="6"/>
+      <c r="A155" t="s">
+        <v>212</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="6"/>
-      <c r="B156" s="6"/>
+      <c r="A156" t="s">
+        <v>213</v>
+      </c>
+      <c r="B156" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="6"/>
-      <c r="B157" s="6"/>
+      <c r="A157" t="s">
+        <v>215</v>
+      </c>
+      <c r="B157" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="6"/>
-      <c r="B158" s="6"/>
+      <c r="A158" t="s">
+        <v>217</v>
+      </c>
+      <c r="B158" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="6"/>
-      <c r="B159" s="6"/>
+      <c r="A159" t="s">
+        <v>218</v>
+      </c>
+      <c r="B159" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="6"/>
-      <c r="B160" s="6"/>
+      <c r="A160" t="s">
+        <v>220</v>
+      </c>
+      <c r="B160" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>222</v>
+      </c>
+      <c r="B161" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>224</v>
+      </c>
+      <c r="B162" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>226</v>
+      </c>
+      <c r="B163" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>227</v>
+      </c>
+      <c r="B164" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>229</v>
+      </c>
+      <c r="B165" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>231</v>
+      </c>
+      <c r="B166" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>310</v>
+      </c>
+      <c r="B167" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>232</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>234</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>235</v>
+      </c>
+      <c r="B170" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>236</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>237</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>238</v>
+      </c>
+      <c r="B173" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>240</v>
+      </c>
+      <c r="B174" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>242</v>
+      </c>
+      <c r="B175" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>243</v>
+      </c>
+      <c r="B176" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>244</v>
+      </c>
+      <c r="B177" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>245</v>
+      </c>
+      <c r="B178" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>246</v>
+      </c>
+      <c r="B179" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>247</v>
+      </c>
+      <c r="B180" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>248</v>
+      </c>
+      <c r="B181" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>249</v>
+      </c>
+      <c r="B182" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>250</v>
+      </c>
+      <c r="B183" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>252</v>
+      </c>
+      <c r="B184" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>253</v>
+      </c>
+      <c r="B185" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>254</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>255</v>
+      </c>
+      <c r="B187" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>257</v>
+      </c>
+      <c r="B188" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>258</v>
+      </c>
+      <c r="B189" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>259</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>260</v>
+      </c>
+      <c r="B191" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>262</v>
+      </c>
+      <c r="B192" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>263</v>
+      </c>
+      <c r="B193" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>264</v>
+      </c>
+      <c r="B194" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B195" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>267</v>
+      </c>
+      <c r="B196" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>268</v>
+      </c>
+      <c r="B197" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>269</v>
+      </c>
+      <c r="B198" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>271</v>
+      </c>
+      <c r="B199" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>272</v>
+      </c>
+      <c r="B200" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>274</v>
+      </c>
+      <c r="B201" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>275</v>
+      </c>
+      <c r="B202" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>277</v>
+      </c>
+      <c r="B203" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>279</v>
+      </c>
+      <c r="B204" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>280</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>281</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>283</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>82</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>284</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>285</v>
+      </c>
+      <c r="B210" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>287</v>
+      </c>
+      <c r="B211" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>313</v>
+      </c>
+      <c r="B212" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>288</v>
+      </c>
+      <c r="B213" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>290</v>
+      </c>
+      <c r="B214" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>292</v>
+      </c>
+      <c r="B215" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>293</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>294</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>296</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>297</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>298</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>300</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>301</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>302</v>
+      </c>
+      <c r="B223" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>303</v>
+      </c>
+      <c r="B224" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>304</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>306</v>
+      </c>
+      <c r="B226" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>307</v>
+      </c>
+      <c r="B227" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>308</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>309</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>299</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B153" r:id="rId1" display="https://saccess.nic/" xr:uid="{51FF1BCE-873B-4803-8820-15C160B4CF91}"/>
+    <hyperlink ref="B168" r:id="rId2" display="https://saccess.nic/" xr:uid="{97405B90-76D1-4859-963D-BD21D1352833}"/>
+    <hyperlink ref="B210" r:id="rId3" display="https://saccess.nic/" xr:uid="{CEEE7ADD-3E54-4127-A250-F0C0984DC727}"/>
+    <hyperlink ref="B169" r:id="rId4" display="https://saccess.nic/" xr:uid="{F6051EEE-BD55-4E15-9B66-843785F2A81D}"/>
+    <hyperlink ref="B170" r:id="rId5" display="https://saccess.nic/" xr:uid="{0EB56D92-63FB-409E-9DF9-17227C987F21}"/>
+    <hyperlink ref="B211" r:id="rId6" display="https://saccess.nic/" xr:uid="{0F5C68CE-7D94-4329-ABE5-97922EC6CCAF}"/>
+    <hyperlink ref="B212" r:id="rId7" display="https://saccess.nic/" xr:uid="{07337387-67F0-42F9-93CA-411B096EC5EB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>